<commit_message>
chore(game): update to 5.10
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -599,7 +599,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>5.10</t>
         </is>
       </c>
     </row>
@@ -1607,7 +1607,7 @@
     <row r="42">
       <c r="A42" s="50" t="inlineStr">
         <is>
-          <t>This product is not yet available in game version 5.00 but was added in 5.50.</t>
+          <t>This product is not yet available in game version 5.10 but was added in 5.50.</t>
         </is>
       </c>
       <c r="C42" s="4" t="n"/>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="D100" s="34" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 5.00 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 5.10 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -12795,7 +12795,7 @@
       </c>
       <c r="D172" s="34" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 5.00 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 5.10 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>
@@ -14085,7 +14085,7 @@
       </c>
       <c r="D2" s="34" t="inlineStr">
         <is>
-          <t>This technology is outdated in game version 5.00 as it was changed in 5.50.</t>
+          <t>This technology is outdated in game version 5.10 as it was changed in 5.50.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(game): update to 5.50
</commit_message>
<xml_diff>
--- a/Pi.xlsx
+++ b/Pi.xlsx
@@ -48,7 +48,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill/>
     </fill>
@@ -83,11 +83,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00cdb3ff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -132,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -179,29 +174,25 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -599,7 +590,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>5.10</t>
+          <t>5.50</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1201,7 @@
       <c r="B3" t="n">
         <v>91860</v>
       </c>
-      <c r="C3" s="49" t="n">
+      <c r="C3" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
@@ -1241,7 +1232,7 @@
       <c r="B6" t="n">
         <v>91860</v>
       </c>
-      <c r="C6" s="49" t="n">
+      <c r="C6" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
@@ -1272,7 +1263,7 @@
       <c r="B9" t="n">
         <v>91860</v>
       </c>
-      <c r="C9" s="49" t="n">
+      <c r="C9" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
@@ -1303,7 +1294,7 @@
       <c r="B12" t="n">
         <v>91860</v>
       </c>
-      <c r="C12" s="49" t="n">
+      <c r="C12" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D12" t="n">
@@ -1334,7 +1325,7 @@
       <c r="B15" t="n">
         <v>91860</v>
       </c>
-      <c r="C15" s="49" t="n">
+      <c r="C15" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D15" t="n">
@@ -1365,7 +1356,7 @@
       <c r="B18" t="n">
         <v>91860</v>
       </c>
-      <c r="C18" s="49" t="n">
+      <c r="C18" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D18" t="n">
@@ -1396,7 +1387,7 @@
       <c r="B21" t="n">
         <v>91860</v>
       </c>
-      <c r="C21" s="49" t="n">
+      <c r="C21" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D21" t="n">
@@ -1427,7 +1418,7 @@
       <c r="B24" t="n">
         <v>91860</v>
       </c>
-      <c r="C24" s="49" t="n">
+      <c r="C24" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D24" t="n">
@@ -1458,7 +1449,7 @@
       <c r="B27" t="n">
         <v>91860</v>
       </c>
-      <c r="C27" s="49" t="n">
+      <c r="C27" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D27" t="n">
@@ -1489,7 +1480,7 @@
       <c r="B30" t="n">
         <v>91860</v>
       </c>
-      <c r="C30" s="49" t="n">
+      <c r="C30" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D30" t="n">
@@ -1520,7 +1511,7 @@
       <c r="B33" t="n">
         <v>91860</v>
       </c>
-      <c r="C33" s="49" t="n">
+      <c r="C33" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D33" t="n">
@@ -1551,7 +1542,7 @@
       <c r="B36" t="n">
         <v>91860</v>
       </c>
-      <c r="C36" s="49" t="n">
+      <c r="C36" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D36" t="n">
@@ -1582,7 +1573,7 @@
       <c r="B39" t="n">
         <v>91860</v>
       </c>
-      <c r="C39" s="49" t="n">
+      <c r="C39" s="48" t="n">
         <v>1</v>
       </c>
       <c r="D39" t="n">
@@ -1605,18 +1596,25 @@
       <c r="C41" s="4" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="50" t="inlineStr">
-        <is>
-          <t>This product is not yet available in game version 5.10 but was added in 5.50.</t>
-        </is>
-      </c>
-      <c r="C42" s="4" t="n"/>
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="n">
+        <v>91860</v>
+      </c>
+      <c r="C42" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2154</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1999941</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="28">
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A26:C26"/>
@@ -1636,7 +1634,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A42:E42"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D29:E29"/>
@@ -4265,11 +4262,7 @@
       <c r="C100" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D100" s="34" t="inlineStr">
-        <is>
-          <t>This technology is outdated in game version 5.10 as it was changed in 5.50.</t>
-        </is>
-      </c>
+      <c r="D100" s="16" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4284,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="19" t="n">
-        <v>179.9986267089844</v>
+        <v>239.9983520507812</v>
       </c>
     </row>
     <row r="102">
@@ -4297,10 +4290,10 @@
         <v>79741</v>
       </c>
       <c r="C102" s="18" t="n">
-        <v>0.9999990844475098</v>
+        <v>0.9999989827194554</v>
       </c>
       <c r="D102" s="20" t="n">
-        <v>179.9985809326172</v>
+        <v>239.998291015625</v>
       </c>
       <c r="E102" s="17" t="n"/>
       <c r="F102" s="17" t="n"/>
@@ -4321,29 +4314,29 @@
         <v>0.9999984740791831</v>
       </c>
       <c r="D103" s="9" t="n">
-        <v>179.9985504150391</v>
+        <v>239.9982604980469</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="35" t="inlineStr">
+      <c r="A104" s="34" t="inlineStr">
         <is>
           <t>Pure Oxygen Gas Pressurizer</t>
         </is>
       </c>
-      <c r="B104" s="35" t="n">
+      <c r="B104" s="34" t="n">
         <v>53523</v>
       </c>
-      <c r="C104" s="36" t="n">
-        <v>0.9999493394288783</v>
-      </c>
-      <c r="D104" s="37" t="n">
-        <v>179.99609375</v>
-      </c>
-      <c r="E104" s="35" t="n"/>
-      <c r="F104" s="35" t="n"/>
-      <c r="G104" s="35" t="n"/>
-      <c r="H104" s="35" t="n"/>
-      <c r="I104" s="35" t="n"/>
+      <c r="C104" s="35" t="n">
+        <v>0.9999496446130417</v>
+      </c>
+      <c r="D104" s="36" t="n">
+        <v>239.9953308105469</v>
+      </c>
+      <c r="E104" s="34" t="n"/>
+      <c r="F104" s="34" t="n"/>
+      <c r="G104" s="34" t="n"/>
+      <c r="H104" s="34" t="n"/>
+      <c r="I104" s="34" t="n"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr"/>
@@ -6233,18 +6226,18 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="35" t="inlineStr">
+      <c r="A62" s="34" t="inlineStr">
         <is>
           <t>Free Electron Refractor</t>
         </is>
       </c>
-      <c r="B62" s="35" t="n">
+      <c r="B62" s="34" t="n">
         <v>91149</v>
       </c>
-      <c r="C62" s="36" t="n">
+      <c r="C62" s="35" t="n">
         <v>0.9999765915040814</v>
       </c>
-      <c r="D62" s="37" t="n">
+      <c r="D62" s="36" t="n">
         <v>27.99971961975098</v>
       </c>
       <c r="E62" s="24" t="n">
@@ -6253,9 +6246,9 @@
       <c r="F62" s="24" t="n">
         <v>2.100002765655518</v>
       </c>
-      <c r="G62" s="35" t="n"/>
-      <c r="H62" s="35" t="n"/>
-      <c r="I62" s="35" t="n"/>
+      <c r="G62" s="34" t="n"/>
+      <c r="H62" s="34" t="n"/>
+      <c r="I62" s="34" t="n"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
@@ -6751,29 +6744,29 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="35" t="inlineStr">
+      <c r="A88" s="34" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B88" s="35" t="n">
+      <c r="B88" s="34" t="n">
         <v>3014</v>
       </c>
-      <c r="C88" s="36" t="n">
+      <c r="C88" s="35" t="n">
         <v>0.2393532220868545</v>
       </c>
       <c r="D88" s="24" t="n">
         <v>7.999974250793457</v>
       </c>
-      <c r="E88" s="37" t="n">
+      <c r="E88" s="36" t="n">
         <v>6.08595609664917</v>
       </c>
-      <c r="F88" s="37" t="n">
+      <c r="F88" s="36" t="n">
         <v>6.003260612487793</v>
       </c>
-      <c r="G88" s="35" t="n"/>
-      <c r="H88" s="35" t="n"/>
-      <c r="I88" s="35" t="n"/>
+      <c r="G88" s="34" t="n"/>
+      <c r="H88" s="34" t="n"/>
+      <c r="I88" s="34" t="n"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -7046,29 +7039,29 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="35" t="inlineStr">
+      <c r="A102" s="34" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B102" s="35" t="n">
+      <c r="B102" s="34" t="n">
         <v>3014</v>
       </c>
-      <c r="C102" s="36" t="n">
+      <c r="C102" s="35" t="n">
         <v>0.3009311425696053</v>
       </c>
       <c r="D102" s="24" t="n">
         <v>11.99998664855957</v>
       </c>
-      <c r="E102" s="37" t="n">
+      <c r="E102" s="36" t="n">
         <v>7.293200492858887</v>
       </c>
-      <c r="F102" s="37" t="n">
+      <c r="F102" s="36" t="n">
         <v>5.142772197723389</v>
       </c>
-      <c r="G102" s="35" t="n"/>
-      <c r="H102" s="35" t="n"/>
-      <c r="I102" s="35" t="n"/>
+      <c r="G102" s="34" t="n"/>
+      <c r="H102" s="34" t="n"/>
+      <c r="I102" s="34" t="n"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr"/>
@@ -7341,29 +7334,29 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="35" t="inlineStr">
+      <c r="A116" s="34" t="inlineStr">
         <is>
           <t>Gamma Ray Accelerator</t>
         </is>
       </c>
-      <c r="B116" s="35" t="n">
+      <c r="B116" s="34" t="n">
         <v>3014</v>
       </c>
-      <c r="C116" s="36" t="n">
+      <c r="C116" s="35" t="n">
         <v>0.2700637885284971</v>
       </c>
       <c r="D116" s="24" t="n">
         <v>11.99998664855957</v>
       </c>
-      <c r="E116" s="37" t="n">
+      <c r="E116" s="36" t="n">
         <v>30.73297739028931</v>
       </c>
-      <c r="F116" s="37" t="n">
+      <c r="F116" s="36" t="n">
         <v>10.14277935028076</v>
       </c>
-      <c r="G116" s="35" t="n"/>
-      <c r="H116" s="35" t="n"/>
-      <c r="I116" s="35" t="n"/>
+      <c r="G116" s="34" t="n"/>
+      <c r="H116" s="34" t="n"/>
+      <c r="I116" s="34" t="n"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr"/>
@@ -7399,7 +7392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8098,18 +8091,18 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="35" t="inlineStr">
+      <c r="A34" s="34" t="inlineStr">
         <is>
           <t>Boundless Gills</t>
         </is>
       </c>
-      <c r="B34" s="35" t="n">
+      <c r="B34" s="34" t="n">
         <v>95566</v>
       </c>
-      <c r="C34" s="36" t="n">
+      <c r="C34" s="35" t="n">
         <v>0.9999561090701528</v>
       </c>
-      <c r="D34" s="37" t="n">
+      <c r="D34" s="36" t="n">
         <v>27.99951934814453</v>
       </c>
       <c r="E34" s="24" t="n">
@@ -8118,9 +8111,9 @@
       <c r="F34" s="24" t="n">
         <v>2.100002765655518</v>
       </c>
-      <c r="G34" s="35" t="n"/>
-      <c r="H34" s="35" t="n"/>
-      <c r="I34" s="35" t="n"/>
+      <c r="G34" s="34" t="n"/>
+      <c r="H34" s="34" t="n"/>
+      <c r="I34" s="34" t="n"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -8166,52 +8159,52 @@
       </c>
       <c r="B37" s="14" t="inlineStr"/>
       <c r="C37" s="15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="16" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Vibrant Iris</t>
+          <t>Chromatic Cornea</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>49936</v>
+        <v>2699</v>
       </c>
       <c r="C38" s="8" t="n">
-        <v>0.9966655828216965</v>
+        <v>0.989701759459199</v>
       </c>
       <c r="D38" s="9" t="n">
-        <v>69.97747802734375</v>
+        <v>69.95418548583984</v>
       </c>
       <c r="E38" s="9" t="n">
-        <v/>
+        <v>94.8948860168457</v>
       </c>
       <c r="F38" s="9" t="n">
-        <v>0.2985389530658722</v>
+        <v>0.2835780680179596</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="17" t="inlineStr">
         <is>
-          <t>Chromatic Pupil</t>
+          <t>Heavenly Fluids</t>
         </is>
       </c>
       <c r="B39" s="17" t="n">
-        <v>69684</v>
+        <v>7012</v>
       </c>
       <c r="C39" s="18" t="n">
-        <v>0.9944162540760497</v>
+        <v>0.9868392572241929</v>
       </c>
       <c r="D39" s="20" t="n">
-        <v>69.95756530761719</v>
+        <v>69.99435424804688</v>
       </c>
       <c r="E39" s="20" t="n">
-        <v/>
+        <v>94.88345384597778</v>
       </c>
       <c r="F39" s="20" t="n">
-        <v>0.2980560660362244</v>
+        <v>0.2720390856266022</v>
       </c>
       <c r="G39" s="17" t="n"/>
       <c r="H39" s="17" t="n"/>
@@ -8220,45 +8213,45 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Translucent Iris</t>
+          <t>Vibrant Iris</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>41731</v>
+        <v>78180</v>
       </c>
       <c r="C40" s="8" t="n">
-        <v>0.9941467186673333</v>
+        <v>0.9859123871135645</v>
       </c>
       <c r="D40" s="9" t="n">
-        <v/>
+        <v>69.7569580078125</v>
       </c>
       <c r="E40" s="9" t="n">
-        <v>94.92594003677368</v>
+        <v>94.86348628997803</v>
       </c>
       <c r="F40" s="9" t="n">
-        <v>0.2952427864074707</v>
+        <v>0.2948956787586212</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="17" t="inlineStr">
         <is>
-          <t>Translucent Cornea</t>
+          <t>Vibrant Cornea</t>
         </is>
       </c>
       <c r="B41" s="17" t="n">
-        <v>54394</v>
+        <v>3014</v>
       </c>
       <c r="C41" s="18" t="n">
-        <v>0.9926566456291257</v>
+        <v>0.648808354180579</v>
       </c>
       <c r="D41" s="20" t="n">
-        <v>69.95663452148438</v>
-      </c>
-      <c r="E41" s="20" t="n">
-        <v/>
+        <v>60.28554916381836</v>
+      </c>
+      <c r="E41" s="19" t="n">
+        <v>94.99987363815308</v>
       </c>
       <c r="F41" s="20" t="n">
-        <v>0.2962136566638947</v>
+        <v>0.2146597355604172</v>
       </c>
       <c r="G41" s="17" t="n"/>
       <c r="H41" s="17" t="n"/>
@@ -8267,193 +8260,52 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Vibrant Retina</t>
+          <t>Vibrant Fluids</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>12603</v>
+        <v>96019</v>
       </c>
       <c r="C42" s="8" t="n">
-        <v>0.992518774938806</v>
+        <v>0.3543848012396342</v>
       </c>
       <c r="D42" s="9" t="n">
-        <v>69.94647979736328</v>
+        <v>69.2298583984375</v>
       </c>
       <c r="E42" s="9" t="n">
-        <v/>
-      </c>
-      <c r="F42" s="9" t="n">
-        <v>0.297077476978302</v>
+        <v>75.4543662071228</v>
+      </c>
+      <c r="F42" s="19" t="n">
+        <v>0.299999475479126</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="17" t="inlineStr">
-        <is>
-          <t>Sleepless Iris</t>
-        </is>
-      </c>
-      <c r="B43" s="17" t="n">
-        <v>2674</v>
-      </c>
-      <c r="C43" s="18" t="n">
-        <v>0.992226300298482</v>
-      </c>
-      <c r="D43" s="20" t="n">
-        <v>69.92471313476562</v>
-      </c>
-      <c r="E43" s="20" t="n">
-        <v/>
-      </c>
-      <c r="F43" s="20" t="n">
-        <v>0.2989324331283569</v>
-      </c>
-      <c r="G43" s="17" t="n"/>
-      <c r="H43" s="17" t="n"/>
-      <c r="I43" s="17" t="n"/>
+      <c r="A43" s="34" t="inlineStr">
+        <is>
+          <t>Translucent Pupil</t>
+        </is>
+      </c>
+      <c r="B43" s="34" t="n">
+        <v>95159</v>
+      </c>
+      <c r="C43" s="35" t="n">
+        <v>0.3465612198827304</v>
+      </c>
+      <c r="D43" s="24" t="n">
+        <v>69.9996337890625</v>
+      </c>
+      <c r="E43" s="36" t="n">
+        <v>75.32020807266235</v>
+      </c>
+      <c r="F43" s="36" t="n">
+        <v>0.2122865915298462</v>
+      </c>
+      <c r="G43" s="34" t="n"/>
+      <c r="H43" s="34" t="n"/>
+      <c r="I43" s="34" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Vibrant Lens</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>11278</v>
-      </c>
-      <c r="C44" s="8" t="n">
-        <v>0.9920887377651073</v>
-      </c>
-      <c r="D44" s="9" t="n">
-        <v>69.92576599121094</v>
-      </c>
-      <c r="E44" s="9" t="n">
-        <v/>
-      </c>
-      <c r="F44" s="9" t="n">
-        <v>0.2986758351325989</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="17" t="inlineStr">
-        <is>
-          <t>Chromatic Retina</t>
-        </is>
-      </c>
-      <c r="B45" s="17" t="n">
-        <v>37541</v>
-      </c>
-      <c r="C45" s="18" t="n">
-        <v>0.9914711364248507</v>
-      </c>
-      <c r="D45" s="20" t="n">
-        <v/>
-      </c>
-      <c r="E45" s="20" t="n">
-        <v>94.96780633926392</v>
-      </c>
-      <c r="F45" s="20" t="n">
-        <v>0.2858711779117584</v>
-      </c>
-      <c r="G45" s="17" t="n"/>
-      <c r="H45" s="17" t="n"/>
-      <c r="I45" s="17" t="n"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Chromatic Aperture</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>50259</v>
-      </c>
-      <c r="C46" s="8" t="n">
-        <v>0.9913160081837883</v>
-      </c>
-      <c r="D46" s="9" t="n">
-        <v>69.99076843261719</v>
-      </c>
-      <c r="E46" s="9" t="n">
-        <v/>
-      </c>
-      <c r="F46" s="9" t="n">
-        <v>0.2913256287574768</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="17" t="inlineStr">
-        <is>
-          <t>Vibrant Cornea</t>
-        </is>
-      </c>
-      <c r="B47" s="17" t="n">
-        <v>39397</v>
-      </c>
-      <c r="C47" s="18" t="n">
-        <v>0.976419302131486</v>
-      </c>
-      <c r="D47" s="20" t="n">
-        <v/>
-      </c>
-      <c r="E47" s="19" t="n">
-        <v>94.99930143356323</v>
-      </c>
-      <c r="F47" s="20" t="n">
-        <v>0.252625435590744</v>
-      </c>
-      <c r="G47" s="17" t="n"/>
-      <c r="H47" s="17" t="n"/>
-      <c r="I47" s="17" t="n"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Vibrant Mirror</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>57743</v>
-      </c>
-      <c r="C48" s="8" t="n">
-        <v>0.973411607280754</v>
-      </c>
-      <c r="D48" s="19" t="n">
-        <v>69.99954986572266</v>
-      </c>
-      <c r="E48" s="9" t="n">
-        <v/>
-      </c>
-      <c r="F48" s="9" t="n">
-        <v>0.2707534730434418</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="35" t="inlineStr">
-        <is>
-          <t>Vibrant Fluids</t>
-        </is>
-      </c>
-      <c r="B49" s="35" t="n">
-        <v>96019</v>
-      </c>
-      <c r="C49" s="36" t="n">
-        <v>0.07136355988009535</v>
-      </c>
-      <c r="D49" s="37" t="n">
-        <v/>
-      </c>
-      <c r="E49" s="37" t="n">
-        <v>75.4543662071228</v>
-      </c>
-      <c r="F49" s="24" t="n">
-        <v>0.299999475479126</v>
-      </c>
-      <c r="G49" s="35" t="n"/>
-      <c r="H49" s="35" t="n"/>
-      <c r="I49" s="35" t="n"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr"/>
+      <c r="A44" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -10646,16 +10498,16 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="38" t="inlineStr">
+      <c r="A84" s="37" t="inlineStr">
         <is>
           <t>Upgrade (1)</t>
         </is>
       </c>
-      <c r="B84" s="38" t="inlineStr"/>
-      <c r="C84" s="39" t="n">
+      <c r="B84" s="37" t="inlineStr"/>
+      <c r="C84" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="D84" s="40" t="inlineStr"/>
+      <c r="D84" s="39" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -10669,7 +10521,7 @@
       <c r="C85" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D85" s="41" t="n">
+      <c r="D85" s="40" t="n">
         <v>1</v>
       </c>
       <c r="E85" s="9" t="n">
@@ -10678,36 +10530,36 @@
       <c r="F85" s="9" t="n">
         <v/>
       </c>
-      <c r="G85" s="41" t="n">
+      <c r="G85" s="40" t="n">
         <v>199.9960780143738</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="42" t="inlineStr">
+      <c r="A86" s="41" t="inlineStr">
         <is>
           <t>Tertiary Injector Plugs</t>
         </is>
       </c>
-      <c r="B86" s="42" t="n">
+      <c r="B86" s="41" t="n">
         <v>66503</v>
       </c>
-      <c r="C86" s="43" t="n">
+      <c r="C86" s="42" t="n">
         <v>0.9638186662144554</v>
       </c>
-      <c r="D86" s="44" t="n">
-        <v/>
-      </c>
-      <c r="E86" s="44" t="n">
+      <c r="D86" s="43" t="n">
+        <v/>
+      </c>
+      <c r="E86" s="43" t="n">
         <v>196.2135009765625</v>
       </c>
-      <c r="F86" s="44" t="n">
-        <v/>
-      </c>
-      <c r="G86" s="44" t="n">
+      <c r="F86" s="43" t="n">
+        <v/>
+      </c>
+      <c r="G86" s="43" t="n">
         <v>196.5467929840088</v>
       </c>
-      <c r="H86" s="42" t="n"/>
-      <c r="I86" s="42" t="n"/>
+      <c r="H86" s="41" t="n"/>
+      <c r="I86" s="41" t="n"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -10735,31 +10587,31 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="42" t="inlineStr">
+      <c r="A88" s="41" t="inlineStr">
         <is>
           <t>Efficient Coils</t>
         </is>
       </c>
-      <c r="B88" s="42" t="n">
+      <c r="B88" s="41" t="n">
         <v>38522</v>
       </c>
-      <c r="C88" s="43" t="n">
+      <c r="C88" s="42" t="n">
         <v>0.9455232585792177</v>
       </c>
-      <c r="D88" s="44" t="n">
-        <v/>
-      </c>
-      <c r="E88" s="44" t="n">
+      <c r="D88" s="43" t="n">
+        <v/>
+      </c>
+      <c r="E88" s="43" t="n">
         <v>190.1379699707031</v>
       </c>
-      <c r="F88" s="44" t="n">
-        <v/>
-      </c>
-      <c r="G88" s="44" t="n">
+      <c r="F88" s="43" t="n">
+        <v/>
+      </c>
+      <c r="G88" s="43" t="n">
         <v>198.9651203155518</v>
       </c>
-      <c r="H88" s="42" t="n"/>
-      <c r="I88" s="42" t="n"/>
+      <c r="H88" s="41" t="n"/>
+      <c r="I88" s="41" t="n"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -10787,31 +10639,31 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="42" t="inlineStr">
+      <c r="A90" s="41" t="inlineStr">
         <is>
           <t>Lubricated Timing Loom</t>
         </is>
       </c>
-      <c r="B90" s="42" t="n">
+      <c r="B90" s="41" t="n">
         <v>81042</v>
       </c>
-      <c r="C90" s="43" t="n">
+      <c r="C90" s="42" t="n">
         <v>0.5</v>
       </c>
-      <c r="D90" s="44" t="n">
-        <v/>
-      </c>
-      <c r="E90" s="41" t="n">
+      <c r="D90" s="43" t="n">
+        <v/>
+      </c>
+      <c r="E90" s="40" t="n">
         <v>199.9966888427734</v>
       </c>
-      <c r="F90" s="44" t="n">
-        <v/>
-      </c>
-      <c r="G90" s="44" t="n">
-        <v/>
-      </c>
-      <c r="H90" s="42" t="n"/>
-      <c r="I90" s="42" t="n"/>
+      <c r="F90" s="43" t="n">
+        <v/>
+      </c>
+      <c r="G90" s="43" t="n">
+        <v/>
+      </c>
+      <c r="H90" s="41" t="n"/>
+      <c r="I90" s="41" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="21" t="inlineStr">
@@ -10831,7 +10683,7 @@
       <c r="E91" s="23" t="n">
         <v/>
       </c>
-      <c r="F91" s="45" t="n">
+      <c r="F91" s="44" t="n">
         <v>4.999732971191406</v>
       </c>
       <c r="G91" s="23" t="n">
@@ -11299,29 +11151,29 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="35" t="inlineStr">
+      <c r="A113" s="34" t="inlineStr">
         <is>
           <t>Nano-Boosted Core</t>
         </is>
       </c>
-      <c r="B113" s="35" t="n">
+      <c r="B113" s="34" t="n">
         <v>96019</v>
       </c>
-      <c r="C113" s="36" t="n">
+      <c r="C113" s="35" t="n">
         <v>0.6721026498583409</v>
       </c>
-      <c r="D113" s="37" t="n">
+      <c r="D113" s="36" t="n">
         <v>351.1358947753906</v>
       </c>
-      <c r="E113" s="37" t="n">
+      <c r="E113" s="36" t="n">
         <v/>
       </c>
       <c r="F113" s="24" t="n">
         <v>299.9994516372681</v>
       </c>
-      <c r="G113" s="35" t="n"/>
-      <c r="H113" s="35" t="n"/>
-      <c r="I113" s="35" t="n"/>
+      <c r="G113" s="34" t="n"/>
+      <c r="H113" s="34" t="n"/>
+      <c r="I113" s="34" t="n"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr"/>
@@ -12793,11 +12645,7 @@
       <c r="C172" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D172" s="34" t="inlineStr">
-        <is>
-          <t>This technology is outdated in game version 5.10 as it was changed in 5.50.</t>
-        </is>
-      </c>
+      <c r="D172" s="7" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -12809,16 +12657,16 @@
         <v>29093</v>
       </c>
       <c r="C173" s="8" t="n">
-        <v>0.9921309936703081</v>
+        <v>0.9917183869604623</v>
       </c>
       <c r="D173" s="9" t="n">
-        <v>29.74483370780945</v>
+        <v>49.54070448875427</v>
       </c>
       <c r="E173" s="9" t="n">
         <v>24.84856605529785</v>
       </c>
       <c r="F173" s="9" t="n">
-        <v>14.96304702758789</v>
+        <v>17.95196151733398</v>
       </c>
       <c r="G173" s="13" t="n">
         <v>1</v>
@@ -12827,23 +12675,23 @@
     <row r="174">
       <c r="A174" s="10" t="inlineStr">
         <is>
-          <t>Outlawed Oscillating Ion Shaper</t>
+          <t>Banned Energised Plasma Unit</t>
         </is>
       </c>
       <c r="B174" s="10" t="n">
-        <v>24640</v>
+        <v>99050</v>
       </c>
       <c r="C174" s="11" t="n">
-        <v>0.9920820889830231</v>
+        <v>0.9909732760153702</v>
       </c>
       <c r="D174" s="12" t="n">
-        <v>29.67646718025208</v>
+        <v>49.46026206016541</v>
       </c>
       <c r="E174" s="12" t="n">
-        <v>24.94010734558105</v>
+        <v>24.86246871948242</v>
       </c>
       <c r="F174" s="12" t="n">
-        <v>14.93768119812012</v>
+        <v>17.95802879333496</v>
       </c>
       <c r="G174" s="13" t="n">
         <v>1</v>
@@ -12854,23 +12702,23 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Forbidden Advanced Linearity Warp</t>
+          <t>Outlawed Oscillating Ion Shaper</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>6883</v>
+        <v>24640</v>
       </c>
       <c r="C175" s="8" t="n">
-        <v>0.9919042395788934</v>
+        <v>0.990923314911643</v>
       </c>
       <c r="D175" s="9" t="n">
-        <v>29.64625358581543</v>
+        <v>49.41763877868652</v>
       </c>
       <c r="E175" s="9" t="n">
-        <v>24.90845489501953</v>
+        <v>24.94010734558105</v>
       </c>
       <c r="F175" s="9" t="n">
-        <v>14.9869213104248</v>
+        <v>17.91898536682129</v>
       </c>
       <c r="G175" s="13" t="n">
         <v>1</v>
@@ -12879,23 +12727,23 @@
     <row r="176">
       <c r="A176" s="10" t="inlineStr">
         <is>
-          <t>Banned Energised Plasma Unit</t>
+          <t>Forbidden Advanced Linearity Warp</t>
         </is>
       </c>
       <c r="B176" s="10" t="n">
-        <v>99050</v>
+        <v>6883</v>
       </c>
       <c r="C176" s="11" t="n">
-        <v>0.9916777469053119</v>
+        <v>0.99068074819454</v>
       </c>
       <c r="D176" s="12" t="n">
-        <v>29.70014810562134</v>
+        <v>49.36325550079346</v>
       </c>
       <c r="E176" s="12" t="n">
-        <v>24.86246871948242</v>
+        <v>24.90845489501953</v>
       </c>
       <c r="F176" s="12" t="n">
-        <v>14.96771430969238</v>
+        <v>17.98299789428711</v>
       </c>
       <c r="G176" s="13" t="n">
         <v>1</v>
@@ -12913,16 +12761,16 @@
         <v>14876</v>
       </c>
       <c r="C177" s="8" t="n">
-        <v>0.980012780200203</v>
+        <v>0.977984600351439</v>
       </c>
       <c r="D177" s="9" t="n">
-        <v>29.41009998321533</v>
+        <v>48.93817901611328</v>
       </c>
       <c r="E177" s="13" t="n">
         <v>24.99994087219238</v>
       </c>
       <c r="F177" s="9" t="n">
-        <v>14.4850606918335</v>
+        <v>17.3305778503418</v>
       </c>
       <c r="G177" s="13" t="n">
         <v>1</v>
@@ -12938,16 +12786,16 @@
         <v>4754</v>
       </c>
       <c r="C178" s="11" t="n">
-        <v>0.9223657721378795</v>
+        <v>0.9077457643085128</v>
       </c>
       <c r="D178" s="12" t="n">
-        <v>26.26911997795105</v>
+        <v>43.28441619873047</v>
       </c>
       <c r="E178" s="12" t="n">
         <v>24.33263969421387</v>
       </c>
       <c r="F178" s="13" t="n">
-        <v>14.99974632263184</v>
+        <v>17.99967193603516</v>
       </c>
       <c r="G178" s="13" t="n">
         <v>1</v>
@@ -12965,16 +12813,16 @@
         <v>32361</v>
       </c>
       <c r="C179" s="8" t="n">
-        <v>0.5924685549103823</v>
+        <v>0.6251017853907771</v>
       </c>
       <c r="D179" s="13" t="n">
-        <v>29.99959588050842</v>
+        <v>49.99927282333374</v>
       </c>
       <c r="E179" s="9" t="n">
         <v/>
       </c>
       <c r="F179" s="9" t="n">
-        <v>7.743895053863525</v>
+        <v>8.567063331604004</v>
       </c>
       <c r="G179" s="13" t="n">
         <v>1</v>
@@ -13288,29 +13136,29 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="46" t="inlineStr">
+      <c r="A194" s="45" t="inlineStr">
         <is>
           <t>Forsaken Capacitor</t>
         </is>
       </c>
-      <c r="B194" s="46" t="n">
+      <c r="B194" s="45" t="n">
         <v>55029</v>
       </c>
-      <c r="C194" s="47" t="n">
+      <c r="C194" s="46" t="n">
         <v>0.5019393878517006</v>
       </c>
       <c r="D194" s="33" t="n">
         <v>3.999966144561768</v>
       </c>
-      <c r="E194" s="48" t="n">
-        <v/>
-      </c>
-      <c r="F194" s="48" t="n">
+      <c r="E194" s="47" t="n">
+        <v/>
+      </c>
+      <c r="F194" s="47" t="n">
         <v>10.61809062957764</v>
       </c>
-      <c r="G194" s="46" t="n"/>
-      <c r="H194" s="46" t="n"/>
-      <c r="I194" s="46" t="n"/>
+      <c r="G194" s="45" t="n"/>
+      <c r="H194" s="45" t="n"/>
+      <c r="I194" s="45" t="n"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr"/>
@@ -13528,29 +13376,29 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="35" t="inlineStr">
+      <c r="A8" s="34" t="inlineStr">
         <is>
           <t>Faultless Recycler</t>
         </is>
       </c>
-      <c r="B8" s="35" t="n">
+      <c r="B8" s="34" t="n">
         <v>32361</v>
       </c>
-      <c r="C8" s="36" t="n">
+      <c r="C8" s="35" t="n">
         <v>0.2099291858044448</v>
       </c>
-      <c r="D8" s="37" t="n">
+      <c r="D8" s="36" t="n">
         <v>30.36361312866211</v>
       </c>
-      <c r="E8" s="37" t="n">
+      <c r="E8" s="36" t="n">
         <v>15.00709652900696</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>9.999978542327881</v>
       </c>
-      <c r="G8" s="35" t="n"/>
-      <c r="H8" s="35" t="n"/>
-      <c r="I8" s="35" t="n"/>
+      <c r="G8" s="34" t="n"/>
+      <c r="H8" s="34" t="n"/>
+      <c r="I8" s="34" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -14034,7 +13882,7 @@
     <col width="6" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
-    <col width="19" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
     <col width="19" customWidth="1" min="6" max="6"/>
     <col width="5" customWidth="1" min="7" max="7"/>
     <col width="5" customWidth="1" min="8" max="8"/>
@@ -14083,11 +13931,7 @@
       <c r="C2" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="34" t="inlineStr">
-        <is>
-          <t>This technology is outdated in game version 5.10 as it was changed in 5.50.</t>
-        </is>
-      </c>
+      <c r="D2" s="16" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -14105,7 +13949,7 @@
         <v>29.9869179725647</v>
       </c>
       <c r="E3" s="19" t="n">
-        <v>10.00000238418579</v>
+        <v>7.500004768371582</v>
       </c>
       <c r="F3" s="9" t="n">
         <v>29.98335361480713</v>
@@ -14127,7 +13971,7 @@
         <v>29.94859218597412</v>
       </c>
       <c r="E4" s="19" t="n">
-        <v>10.00000238418579</v>
+        <v>7.500004768371582</v>
       </c>
       <c r="F4" s="20" t="n">
         <v>29.95694279670715</v>
@@ -14152,7 +13996,7 @@
         <v>29.92032170295715</v>
       </c>
       <c r="E5" s="19" t="n">
-        <v>10.00000238418579</v>
+        <v>7.500004768371582</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>29.97245788574219</v>
@@ -14174,7 +14018,7 @@
         <v>29.91818785667419</v>
       </c>
       <c r="E6" s="19" t="n">
-        <v>10.00000238418579</v>
+        <v>7.500004768371582</v>
       </c>
       <c r="F6" s="20" t="n">
         <v>29.96772527694702</v>
@@ -14199,36 +14043,36 @@
         <v>29.99942302703857</v>
       </c>
       <c r="E7" s="19" t="n">
-        <v>10.00000238418579</v>
+        <v>7.500004768371582</v>
       </c>
       <c r="F7" s="9" t="n">
         <v>26.86187922954559</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="35" t="inlineStr">
+      <c r="A8" s="34" t="inlineStr">
         <is>
           <t>High Pressure Turbine Controller</t>
         </is>
       </c>
-      <c r="B8" s="35" t="n">
+      <c r="B8" s="34" t="n">
         <v>96019</v>
       </c>
-      <c r="C8" s="36" t="n">
+      <c r="C8" s="35" t="n">
         <v>0.8061205041219637</v>
       </c>
-      <c r="D8" s="37" t="n">
+      <c r="D8" s="36" t="n">
         <v>25.81901550292969</v>
       </c>
       <c r="E8" s="24" t="n">
-        <v>10.00000238418579</v>
+        <v>7.500004768371582</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>29.99997437000275</v>
       </c>
-      <c r="G8" s="35" t="n"/>
-      <c r="H8" s="35" t="n"/>
-      <c r="I8" s="35" t="n"/>
+      <c r="G8" s="34" t="n"/>
+      <c r="H8" s="34" t="n"/>
+      <c r="I8" s="34" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -14728,29 +14572,29 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="35" t="inlineStr">
+      <c r="A16" s="34" t="inlineStr">
         <is>
           <t>Faultless Recycler</t>
         </is>
       </c>
-      <c r="B16" s="35" t="n">
+      <c r="B16" s="34" t="n">
         <v>32361</v>
       </c>
-      <c r="C16" s="36" t="n">
+      <c r="C16" s="35" t="n">
         <v>0.2099282888068533</v>
       </c>
-      <c r="D16" s="37" t="n">
+      <c r="D16" s="36" t="n">
         <v>30.36361312866211</v>
       </c>
-      <c r="E16" s="37" t="n">
+      <c r="E16" s="36" t="n">
         <v>15.00709652900696</v>
       </c>
       <c r="F16" s="24" t="n">
         <v>9.999954700469971</v>
       </c>
-      <c r="G16" s="35" t="n"/>
-      <c r="H16" s="35" t="n"/>
-      <c r="I16" s="35" t="n"/>
+      <c r="G16" s="34" t="n"/>
+      <c r="H16" s="34" t="n"/>
+      <c r="I16" s="34" t="n"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -15067,15 +14911,15 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="35" t="inlineStr">
+      <c r="A33" s="34" t="inlineStr">
         <is>
           <t>Superheated Exhaust</t>
         </is>
       </c>
-      <c r="B33" s="35" t="n">
+      <c r="B33" s="34" t="n">
         <v>46775</v>
       </c>
-      <c r="C33" s="36" t="n">
+      <c r="C33" s="35" t="n">
         <v>0.4285695674210536</v>
       </c>
       <c r="D33" s="24" t="n">
@@ -15084,12 +14928,12 @@
       <c r="E33" s="24" t="n">
         <v>29.99978065490723</v>
       </c>
-      <c r="F33" s="37" t="n">
+      <c r="F33" s="36" t="n">
         <v>20.00000476837158</v>
       </c>
-      <c r="G33" s="35" t="n"/>
-      <c r="H33" s="35" t="n"/>
-      <c r="I33" s="35" t="n"/>
+      <c r="G33" s="34" t="n"/>
+      <c r="H33" s="34" t="n"/>
+      <c r="I33" s="34" t="n"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -15431,25 +15275,25 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="inlineStr">
+      <c r="A18" s="34" t="inlineStr">
         <is>
           <t>Navigation AI Unit from SS Emperor Bayaseb</t>
         </is>
       </c>
-      <c r="B18" s="35" t="n">
+      <c r="B18" s="34" t="n">
         <v>88814</v>
       </c>
-      <c r="C18" s="36" t="n">
+      <c r="C18" s="35" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="24" t="n">
         <v>19.9999988079071</v>
       </c>
-      <c r="E18" s="35" t="n"/>
-      <c r="F18" s="35" t="n"/>
-      <c r="G18" s="35" t="n"/>
-      <c r="H18" s="35" t="n"/>
-      <c r="I18" s="35" t="n"/>
+      <c r="E18" s="34" t="n"/>
+      <c r="F18" s="34" t="n"/>
+      <c r="G18" s="34" t="n"/>
+      <c r="H18" s="34" t="n"/>
+      <c r="I18" s="34" t="n"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>

</xml_diff>